<commit_message>
Final update before submission
</commit_message>
<xml_diff>
--- a/BunTek_roster.xlsx
+++ b/BunTek_roster.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni Projects\BunTek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D4AB761-CD5C-472D-8D3A-3616288BC14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139C1B6E-FEF4-449F-9C29-6D825C7B3A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Team Name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>m.cheong@digipen.edu</t>
+  </si>
+  <si>
+    <t>No Pic, sorry :(</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -148,6 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,16 +458,16 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -479,7 +483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -487,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -495,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -503,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -511,7 +515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -519,16 +523,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="B10" s="5"/>
     </row>
   </sheetData>

</xml_diff>